<commit_message>
SQL & Excel utilities refined
</commit_message>
<xml_diff>
--- a/target/classes/testData/testData.xlsx
+++ b/target/classes/testData/testData.xlsx
@@ -19,7 +19,14 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="0" uniqueCount="0"/>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="2">
+  <si>
+    <t>John Wick</t>
+  </si>
+  <si>
+    <t>James Bond</t>
+  </si>
+</sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
@@ -336,14 +343,37 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B1"/>
+  <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="n">
+        <v>1001.0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" t="n">
+        <v>89.0</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="n">
+        <v>1002.0</v>
+      </c>
+      <c r="B2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" t="n">
+        <v>82.0</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>